<commit_message>
vocabulary updated.  - mimikara oboeru n3 vocab  - Speed Master N3 Vocab
</commit_message>
<xml_diff>
--- a/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
+++ b/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="2482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="2486">
   <si>
     <t>man (male gender)</t>
   </si>
@@ -7460,6 +7460,18 @@
   </si>
   <si>
     <t>to knock over; to defeat</t>
+  </si>
+  <si>
+    <t>ေနသားက်သည္</t>
+  </si>
+  <si>
+    <t>ေနသားက်ေအာင္လုပ္သည္</t>
+  </si>
+  <si>
+    <t>ျမည္သည္</t>
+  </si>
+  <si>
+    <t>ျမည္ေအာင္လုပ္သည္</t>
   </si>
 </sst>
 </file>
@@ -7810,8 +7822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F946"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" topLeftCell="B223" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11057,7 +11069,9 @@
       <c r="D232" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="E232" s="1"/>
+      <c r="E232" s="1" t="s">
+        <v>2484</v>
+      </c>
       <c r="F232" s="1"/>
     </row>
     <row r="233" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -11071,7 +11085,9 @@
       <c r="D233" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="E233" s="1"/>
+      <c r="E233" s="1" t="s">
+        <v>2485</v>
+      </c>
       <c r="F233" s="1"/>
     </row>
     <row r="234" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -14805,7 +14821,9 @@
       <c r="D503" s="1" t="s">
         <v>1362</v>
       </c>
-      <c r="E503" s="1"/>
+      <c r="E503" s="1" t="s">
+        <v>2482</v>
+      </c>
       <c r="F503" s="1"/>
     </row>
     <row r="504" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -14819,7 +14837,9 @@
       <c r="D504" s="1" t="s">
         <v>1364</v>
       </c>
-      <c r="E504" s="1"/>
+      <c r="E504" s="1" t="s">
+        <v>2483</v>
+      </c>
       <c r="F504" s="1"/>
     </row>
     <row r="505" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
memrise-mimikara-oboeru-N3-Vocab.xlsx -> Myanmar Definition added for Part 40. New word list added for Japanese Onomatopoeia (Giongo, Giseigo, Gitaigo) (Sorry! I'll not open yet this one.)
</commit_message>
<xml_diff>
--- a/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
+++ b/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data History" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="2486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="2499">
   <si>
     <t>man (male gender)</t>
   </si>
@@ -7472,13 +7473,52 @@
   </si>
   <si>
     <t>ျမည္ေအာင္လုပ္သည္</t>
+  </si>
+  <si>
+    <t>ျပန္႔ႀကဲေနေသာ</t>
+  </si>
+  <si>
+    <t>စုတ္ၿပဲေနေသာ</t>
+  </si>
+  <si>
+    <t>အလြန္အမင္း</t>
+  </si>
+  <si>
+    <t>ေတာ္ေတာ္ေလး</t>
+  </si>
+  <si>
+    <t>(ေတြးထားတာနဲ႔ ႏိႈင္းယွဥ္ၿပီးေျပာတာ)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Zaw Tun Latt</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Part 40 : Myanmar Definition (#Zawgyi) added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7492,16 +7532,30 @@
       <name val="Zawgyi-One"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -7509,13 +7563,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7820,10 +7897,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K7:K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>2491</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2492</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2493</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2494</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2495</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>2495</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2495</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43368</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2496</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2498</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F946"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B223" workbookViewId="0">
-      <selection activeCell="C231" sqref="C231"/>
+    <sheetView topLeftCell="A622" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7837,7 +8026,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>2497</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>2441</v>
       </c>
@@ -16543,7 +16734,9 @@
       <c r="D628" s="1" t="s">
         <v>1663</v>
       </c>
-      <c r="E628" s="1"/>
+      <c r="E628" s="1" t="s">
+        <v>2486</v>
+      </c>
       <c r="F628" s="1"/>
     </row>
     <row r="629" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -16557,7 +16750,9 @@
       <c r="D629" s="1" t="s">
         <v>1665</v>
       </c>
-      <c r="E629" s="1"/>
+      <c r="E629" s="1" t="s">
+        <v>2487</v>
+      </c>
       <c r="F629" s="1"/>
     </row>
     <row r="630" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -16571,7 +16766,9 @@
       <c r="D630" s="1" t="s">
         <v>1667</v>
       </c>
-      <c r="E630" s="1"/>
+      <c r="E630" s="1" t="s">
+        <v>2488</v>
+      </c>
       <c r="F630" s="1"/>
     </row>
     <row r="631" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -16627,7 +16824,9 @@
       <c r="D634" s="1" t="s">
         <v>1675</v>
       </c>
-      <c r="E634" s="1"/>
+      <c r="E634" s="1" t="s">
+        <v>2489</v>
+      </c>
       <c r="F634" s="1"/>
     </row>
     <row r="635" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -16641,7 +16840,9 @@
       <c r="D635" s="1" t="s">
         <v>1675</v>
       </c>
-      <c r="E635" s="1"/>
+      <c r="E635" s="1" t="s">
+        <v>2489</v>
+      </c>
       <c r="F635" s="1"/>
     </row>
     <row r="636" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -16655,7 +16856,9 @@
       <c r="D636" s="1" t="s">
         <v>1678</v>
       </c>
-      <c r="E636" s="1"/>
+      <c r="E636" s="1" t="s">
+        <v>2490</v>
+      </c>
       <c r="F636" s="1"/>
     </row>
     <row r="637" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
# missing word is corrected memrise-mimikara-oboeru-N3-Vocab.xlsx
</commit_message>
<xml_diff>
--- a/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
+++ b/created/memrise-mimikara-oboeru-N3-Vocab.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Data History" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2720" uniqueCount="2502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="2503">
   <si>
     <t>man (male gender)</t>
   </si>
@@ -6941,9 +6941,6 @@
     <t>energy</t>
   </si>
   <si>
-    <t>エネルジー</t>
-  </si>
-  <si>
     <t>digital</t>
   </si>
   <si>
@@ -7521,6 +7518,12 @@
   </si>
   <si>
     <t>それとも</t>
+  </si>
+  <si>
+    <t>エネルギー</t>
+  </si>
+  <si>
+    <t>Part 56 : Missing Katakana is corrected</t>
   </si>
 </sst>
 </file>
@@ -7908,8 +7911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7921,16 +7924,16 @@
   <sheetData>
     <row r="2" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>2489</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2490</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2491</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2492</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2493</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7938,13 +7941,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>2494</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -7955,10 +7958,10 @@
         <v>43368</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7969,10 +7972,10 @@
         <v>43373</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -7983,17 +7986,25 @@
         <v>43374</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>2500</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43376</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>2494</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>2502</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
@@ -8035,8 +8046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F946"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A929" workbookViewId="0">
-      <selection activeCell="C945" sqref="C945"/>
+    <sheetView topLeftCell="A875" workbookViewId="0">
+      <selection activeCell="C886" sqref="C886"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8051,22 +8062,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2440</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2441</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2442</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>2456</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2457</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2458</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
@@ -9729,7 +9740,7 @@
         <v>328</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="F122" s="1"/>
     </row>
@@ -9745,7 +9756,7 @@
         <v>330</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="F123" s="1"/>
     </row>
@@ -9817,7 +9828,7 @@
         <v>340</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="F128" s="1"/>
     </row>
@@ -9857,7 +9868,7 @@
         <v>359</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="F131" s="1"/>
     </row>
@@ -9873,7 +9884,7 @@
         <v>361</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="F132" s="1"/>
     </row>
@@ -9889,7 +9900,7 @@
         <v>363</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="F133" s="1"/>
     </row>
@@ -9905,7 +9916,7 @@
         <v>365</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="F134" s="1"/>
     </row>
@@ -9921,7 +9932,7 @@
         <v>367</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="F135" s="1"/>
     </row>
@@ -9937,7 +9948,7 @@
         <v>369</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="F136" s="1"/>
     </row>
@@ -9953,7 +9964,7 @@
         <v>371</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="F137" s="1"/>
     </row>
@@ -9966,10 +9977,10 @@
         <v>373</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="F138" s="1"/>
     </row>
@@ -9985,7 +9996,7 @@
         <v>374</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="F139" s="1"/>
     </row>
@@ -10001,7 +10012,7 @@
         <v>376</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="F140" s="1"/>
     </row>
@@ -10017,7 +10028,7 @@
         <v>378</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="F141" s="1"/>
     </row>
@@ -10033,7 +10044,7 @@
         <v>380</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="F142" s="1"/>
     </row>
@@ -10049,7 +10060,7 @@
         <v>382</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="F143" s="1"/>
     </row>
@@ -10065,7 +10076,7 @@
         <v>384</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="F144" s="1"/>
     </row>
@@ -10081,7 +10092,7 @@
         <v>386</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="F145" s="1"/>
     </row>
@@ -10135,7 +10146,7 @@
         <v>405</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="F149" s="1"/>
     </row>
@@ -10151,7 +10162,7 @@
         <v>407</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="F150" s="1"/>
     </row>
@@ -10181,7 +10192,7 @@
         <v>411</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="F152" s="1"/>
     </row>
@@ -10281,7 +10292,7 @@
         <v>425</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="F159" s="1"/>
     </row>
@@ -11285,7 +11296,7 @@
         <v>627</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="F232" s="1"/>
     </row>
@@ -11301,7 +11312,7 @@
         <v>629</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="F233" s="1"/>
     </row>
@@ -11632,7 +11643,7 @@
         <v>690</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="E257" s="1"/>
       <c r="F257" s="1"/>
@@ -11782,7 +11793,7 @@
         <v>724</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="E268" s="1"/>
       <c r="F268" s="1"/>
@@ -11799,7 +11810,7 @@
         <v>725</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="F269" s="1"/>
     </row>
@@ -13290,10 +13301,10 @@
     <row r="378" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A378" s="1"/>
       <c r="B378" s="1" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C378" s="1" t="s">
         <v>2435</v>
-      </c>
-      <c r="C378" s="1" t="s">
-        <v>2436</v>
       </c>
       <c r="D378" s="1" t="s">
         <v>1024</v>
@@ -13374,7 +13385,7 @@
     <row r="384" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A384" s="1"/>
       <c r="B384" s="1" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="C384" s="1" t="s">
         <v>1036</v>
@@ -13594,10 +13605,10 @@
     <row r="400" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A400" s="1"/>
       <c r="B400" s="1" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="D400" s="1" t="s">
         <v>1078</v>
@@ -13928,7 +13939,7 @@
         <v>1148</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="E424" s="1"/>
       <c r="F424" s="1"/>
@@ -14563,14 +14574,14 @@
         <v>1274</v>
       </c>
       <c r="E470" s="1" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="F470" s="1"/>
     </row>
     <row r="471" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A471" s="1"/>
       <c r="B471" s="1" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>1277</v>
@@ -14607,7 +14618,7 @@
         <v>1280</v>
       </c>
       <c r="E473" s="1" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="F473" s="1"/>
     </row>
@@ -14623,7 +14634,7 @@
         <v>1282</v>
       </c>
       <c r="E474" s="1" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="F474" s="1"/>
     </row>
@@ -14639,7 +14650,7 @@
         <v>1284</v>
       </c>
       <c r="E475" s="1" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="F475" s="1"/>
     </row>
@@ -14655,7 +14666,7 @@
         <v>1286</v>
       </c>
       <c r="E476" s="1" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="F476" s="1"/>
     </row>
@@ -14671,7 +14682,7 @@
         <v>1288</v>
       </c>
       <c r="E477" s="1" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="F477" s="1"/>
     </row>
@@ -14701,7 +14712,7 @@
         <v>1292</v>
       </c>
       <c r="E479" s="1" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="F479" s="1"/>
     </row>
@@ -14717,7 +14728,7 @@
         <v>1294</v>
       </c>
       <c r="E480" s="1" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="F480" s="1"/>
     </row>
@@ -14733,7 +14744,7 @@
         <v>1296</v>
       </c>
       <c r="E481" s="1" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="F481" s="1"/>
     </row>
@@ -14759,7 +14770,7 @@
         <v>1311</v>
       </c>
       <c r="E483" s="1" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="F483" s="1"/>
     </row>
@@ -15037,7 +15048,7 @@
         <v>1362</v>
       </c>
       <c r="E503" s="1" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="F503" s="1"/>
     </row>
@@ -15053,7 +15064,7 @@
         <v>1364</v>
       </c>
       <c r="E504" s="1" t="s">
-        <v>2482</v>
+        <v>2481</v>
       </c>
       <c r="F504" s="1"/>
     </row>
@@ -16759,7 +16770,7 @@
         <v>1663</v>
       </c>
       <c r="E628" s="1" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="F628" s="1"/>
     </row>
@@ -16775,7 +16786,7 @@
         <v>1665</v>
       </c>
       <c r="E629" s="1" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="F629" s="1"/>
     </row>
@@ -16791,7 +16802,7 @@
         <v>1667</v>
       </c>
       <c r="E630" s="1" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="F630" s="1"/>
     </row>
@@ -16849,7 +16860,7 @@
         <v>1675</v>
       </c>
       <c r="E634" s="1" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="F634" s="1"/>
     </row>
@@ -16865,7 +16876,7 @@
         <v>1675</v>
       </c>
       <c r="E635" s="1" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="F635" s="1"/>
     </row>
@@ -16881,7 +16892,7 @@
         <v>1678</v>
       </c>
       <c r="E636" s="1" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="F636" s="1"/>
     </row>
@@ -17743,7 +17754,7 @@
         <v>1854</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>2499</v>
+        <v>2498</v>
       </c>
       <c r="D699" s="1" t="s">
         <v>1833</v>
@@ -19608,7 +19619,7 @@
     <row r="835" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A835" s="1"/>
       <c r="B835" s="1" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="C835" s="1" t="s">
         <v>2205</v>
@@ -20309,11 +20320,11 @@
     </row>
     <row r="886" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A886" s="1"/>
-      <c r="B886" s="1" t="s">
-        <v>2308</v>
-      </c>
-      <c r="C886" s="1" t="s">
-        <v>2308</v>
+      <c r="B886" t="s">
+        <v>2501</v>
+      </c>
+      <c r="C886" t="s">
+        <v>2501</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>2307</v>
@@ -20324,13 +20335,13 @@
     <row r="887" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A887" s="1"/>
       <c r="B887" s="1" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="D887" s="1" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E887" s="1"/>
       <c r="F887" s="1"/>
@@ -20338,13 +20349,13 @@
     <row r="888" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A888" s="1"/>
       <c r="B888" s="1" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D888" s="1" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="E888" s="1"/>
       <c r="F888" s="1"/>
@@ -20352,13 +20363,13 @@
     <row r="889" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A889" s="1"/>
       <c r="B889" s="1" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="D889" s="1" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="E889" s="1"/>
       <c r="F889" s="1"/>
@@ -20366,13 +20377,13 @@
     <row r="890" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A890" s="1"/>
       <c r="B890" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="D890" s="1" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="E890" s="1"/>
       <c r="F890" s="1"/>
@@ -20380,13 +20391,13 @@
     <row r="891" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A891" s="1"/>
       <c r="B891" s="1" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="D891" s="1" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="E891" s="1"/>
       <c r="F891" s="1"/>
@@ -20394,13 +20405,13 @@
     <row r="892" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A892" s="1"/>
       <c r="B892" s="1" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="D892" s="1" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="E892" s="1"/>
       <c r="F892" s="1"/>
@@ -20408,13 +20419,13 @@
     <row r="893" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A893" s="1"/>
       <c r="B893" s="1" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="D893" s="1" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="E893" s="1"/>
       <c r="F893" s="1"/>
@@ -20422,7 +20433,7 @@
     <row r="894" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A894" s="1"/>
       <c r="B894" s="1" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C894" s="1" t="s">
         <v>1233</v>
@@ -20436,13 +20447,13 @@
     <row r="895" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A895" s="1"/>
       <c r="B895" s="1" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="D895" s="1" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="E895" s="1"/>
       <c r="F895" s="1"/>
@@ -20450,13 +20461,13 @@
     <row r="896" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A896" s="1"/>
       <c r="B896" s="1" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D896" s="1" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="E896" s="1"/>
       <c r="F896" s="1"/>
@@ -20464,13 +20475,13 @@
     <row r="897" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A897" s="1"/>
       <c r="B897" s="1" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="D897" s="1" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="E897" s="1"/>
       <c r="F897" s="1"/>
@@ -20488,13 +20499,13 @@
     <row r="899" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A899" s="1"/>
       <c r="B899" s="1" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="D899" s="1" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="E899" s="1"/>
       <c r="F899" s="1"/>
@@ -20502,13 +20513,13 @@
     <row r="900" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A900" s="1"/>
       <c r="B900" s="1" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="D900" s="1" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="E900" s="1"/>
       <c r="F900" s="1"/>
@@ -20516,13 +20527,13 @@
     <row r="901" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A901" s="1"/>
       <c r="B901" s="1" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D901" s="1" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="E901" s="1"/>
       <c r="F901" s="1"/>
@@ -20530,13 +20541,13 @@
     <row r="902" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A902" s="1"/>
       <c r="B902" s="1" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="D902" s="1" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="E902" s="1"/>
       <c r="F902" s="1"/>
@@ -20544,13 +20555,13 @@
     <row r="903" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A903" s="1"/>
       <c r="B903" s="1" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="D903" s="1" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="E903" s="1"/>
       <c r="F903" s="1"/>
@@ -20558,13 +20569,13 @@
     <row r="904" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A904" s="1"/>
       <c r="B904" s="1" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="D904" s="1" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="E904" s="1"/>
       <c r="F904" s="1"/>
@@ -20572,13 +20583,13 @@
     <row r="905" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A905" s="1"/>
       <c r="B905" s="1" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="D905" s="1" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="E905" s="1"/>
       <c r="F905" s="1"/>
@@ -20586,13 +20597,13 @@
     <row r="906" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A906" s="1"/>
       <c r="B906" s="1" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="D906" s="1" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="E906" s="1"/>
       <c r="F906" s="1"/>
@@ -20600,13 +20611,13 @@
     <row r="907" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A907" s="1"/>
       <c r="B907" s="1" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D907" s="1" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="E907" s="1"/>
       <c r="F907" s="1"/>
@@ -20614,13 +20625,13 @@
     <row r="908" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A908" s="1"/>
       <c r="B908" s="1" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D908" s="1" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="E908" s="1"/>
       <c r="F908" s="1"/>
@@ -20628,13 +20639,13 @@
     <row r="909" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A909" s="1"/>
       <c r="B909" s="1" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="D909" s="1" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="E909" s="1"/>
       <c r="F909" s="1"/>
@@ -20642,13 +20653,13 @@
     <row r="910" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A910" s="1"/>
       <c r="B910" s="1" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="D910" s="1" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="E910" s="1"/>
       <c r="F910" s="1"/>
@@ -20656,13 +20667,13 @@
     <row r="911" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A911" s="1"/>
       <c r="B911" s="1" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="D911" s="1" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="E911" s="1"/>
       <c r="F911" s="1"/>
@@ -20670,13 +20681,13 @@
     <row r="912" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A912" s="1"/>
       <c r="B912" s="1" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D912" s="1" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="E912" s="1"/>
       <c r="F912" s="1"/>
@@ -20684,10 +20695,10 @@
     <row r="913" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A913" s="1"/>
       <c r="B913" s="1" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>1750</v>
@@ -20708,13 +20719,13 @@
     <row r="915" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A915" s="1"/>
       <c r="B915" s="1" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="C915" s="1" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D915" s="1" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="E915" s="1"/>
       <c r="F915" s="1"/>
@@ -20722,13 +20733,13 @@
     <row r="916" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A916" s="1"/>
       <c r="B916" s="1" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="D916" s="1" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="E916" s="1"/>
       <c r="F916" s="1"/>
@@ -20736,13 +20747,13 @@
     <row r="917" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A917" s="1"/>
       <c r="B917" s="1" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="C917" s="1" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="D917" s="1" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="E917" s="1"/>
       <c r="F917" s="1"/>
@@ -20750,13 +20761,13 @@
     <row r="918" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A918" s="1"/>
       <c r="B918" s="1" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="C918" s="1" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="D918" s="1" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="E918" s="1"/>
       <c r="F918" s="1"/>
@@ -20764,13 +20775,13 @@
     <row r="919" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A919" s="1"/>
       <c r="B919" s="1" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="D919" s="1" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="E919" s="1"/>
       <c r="F919" s="1"/>
@@ -20778,13 +20789,13 @@
     <row r="920" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A920" s="1"/>
       <c r="B920" s="1" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="C920" s="1" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="E920" s="1"/>
       <c r="F920" s="1"/>
@@ -20792,13 +20803,13 @@
     <row r="921" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A921" s="1"/>
       <c r="B921" s="1" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="D921" s="1" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="E921" s="1"/>
       <c r="F921" s="1"/>
@@ -20806,13 +20817,13 @@
     <row r="922" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A922" s="1"/>
       <c r="B922" s="1" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="D922" s="1" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E922" s="1"/>
       <c r="F922" s="1"/>
@@ -20820,13 +20831,13 @@
     <row r="923" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A923" s="1"/>
       <c r="B923" s="1" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="D923" s="1" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E923" s="1"/>
       <c r="F923" s="1"/>
@@ -20834,13 +20845,13 @@
     <row r="924" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A924" s="1"/>
       <c r="B924" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="C924" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="D924" s="1" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E924" s="1"/>
       <c r="F924" s="1"/>
@@ -20848,13 +20859,13 @@
     <row r="925" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A925" s="1"/>
       <c r="B925" s="1" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="C925" s="1" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D925" s="1" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E925" s="1"/>
       <c r="F925" s="1"/>
@@ -20862,13 +20873,13 @@
     <row r="926" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A926" s="1"/>
       <c r="B926" s="1" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D926" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="E926" s="1"/>
       <c r="F926" s="1"/>
@@ -20876,13 +20887,13 @@
     <row r="927" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A927" s="1"/>
       <c r="B927" s="1" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D927" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="E927" s="1"/>
       <c r="F927" s="1"/>
@@ -20890,13 +20901,13 @@
     <row r="928" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A928" s="1"/>
       <c r="B928" s="1" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D928" s="1" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="E928" s="1"/>
       <c r="F928" s="1"/>
@@ -20904,13 +20915,13 @@
     <row r="929" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A929" s="1"/>
       <c r="B929" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="D929" s="1" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="E929" s="1"/>
       <c r="F929" s="1"/>
@@ -20928,13 +20939,13 @@
     <row r="931" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A931" s="1"/>
       <c r="B931" s="1" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="D931" s="1" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="E931" s="1"/>
       <c r="F931" s="1"/>
@@ -20942,13 +20953,13 @@
     <row r="932" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A932" s="1"/>
       <c r="B932" s="1" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="D932" s="1" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="E932" s="1"/>
       <c r="F932" s="1"/>
@@ -20956,13 +20967,13 @@
     <row r="933" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A933" s="1"/>
       <c r="B933" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="C933" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="D933" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="E933" s="1"/>
       <c r="F933" s="1"/>
@@ -20970,13 +20981,13 @@
     <row r="934" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A934" s="1"/>
       <c r="B934" s="1" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="C934" s="1" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="D934" s="1" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="E934" s="1"/>
       <c r="F934" s="1"/>
@@ -20984,13 +20995,13 @@
     <row r="935" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A935" s="1"/>
       <c r="B935" s="1" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="D935" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="E935" s="1"/>
       <c r="F935" s="1"/>
@@ -20998,13 +21009,13 @@
     <row r="936" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A936" s="1"/>
       <c r="B936" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="D936" s="1" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="E936" s="1"/>
       <c r="F936" s="1"/>
@@ -21012,13 +21023,13 @@
     <row r="937" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A937" s="1"/>
       <c r="B937" s="1" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="D937" s="1" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="E937" s="1"/>
       <c r="F937" s="1"/>
@@ -21026,13 +21037,13 @@
     <row r="938" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A938" s="1"/>
       <c r="B938" s="1" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="D938" s="1" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="E938" s="1"/>
       <c r="F938" s="1"/>
@@ -21040,13 +21051,13 @@
     <row r="939" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A939" s="1"/>
       <c r="B939" s="1" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="D939" s="1" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="E939" s="1"/>
       <c r="F939" s="1"/>
@@ -21054,13 +21065,13 @@
     <row r="940" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A940" s="1"/>
       <c r="B940" s="1" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="D940" s="1" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="E940" s="1"/>
       <c r="F940" s="1"/>
@@ -21068,13 +21079,13 @@
     <row r="941" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A941" s="1"/>
       <c r="B941" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="D941" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="E941" s="1"/>
       <c r="F941" s="1"/>
@@ -21082,13 +21093,13 @@
     <row r="942" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A942" s="1"/>
       <c r="B942" s="1" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="D942" s="1" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="E942" s="1"/>
       <c r="F942" s="1"/>
@@ -21096,13 +21107,13 @@
     <row r="943" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A943" s="1"/>
       <c r="B943" s="1" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="D943" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="E943" s="1"/>
       <c r="F943" s="1"/>
@@ -21110,13 +21121,13 @@
     <row r="944" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A944" s="1"/>
       <c r="B944" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="D944" s="1" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="E944" s="1"/>
       <c r="F944" s="1"/>
@@ -21124,13 +21135,13 @@
     <row r="945" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A945" s="1"/>
       <c r="B945" s="1" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>2501</v>
+        <v>2500</v>
       </c>
       <c r="D945" s="1" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="E945" s="1"/>
       <c r="F945" s="1"/>
@@ -21138,13 +21149,13 @@
     <row r="946" spans="1:6" ht="19.8" x14ac:dyDescent="0.6">
       <c r="A946" s="1"/>
       <c r="B946" s="1" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="D946" s="1" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="E946" s="1"/>
       <c r="F946" s="1"/>

</xml_diff>